<commit_message>
ajoute un espace insecable dans l'email dans le fichier excel pour améliorer le test
</commit_message>
<xml_diff>
--- a/test/sample/userBase.xlsx
+++ b/test/sample/userBase.xlsx
@@ -8,9 +8,9 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="utilisateurs" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="zones" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="doc wekan" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="utilisateurs" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="zones" sheetId="2" state="visible" r:id="rId4"/>
+    <sheet name="doc wekan" sheetId="3" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -123,7 +123,7 @@
     <t xml:space="preserve">SQUELBUT</t>
   </si>
   <si>
-    <t xml:space="preserve">raphael.squelbut@shodo.io</t>
+    <t xml:space="preserve"> raphael.squelbut@shodo.io</t>
   </si>
   <si>
     <t xml:space="preserve">signauxfaibles</t>
@@ -844,7 +844,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -857,27 +857,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="165" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -905,6 +889,178 @@
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="ffffff"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="a7a7a7"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="535353"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4f81bd"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="c0504d"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9bbb59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064a2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4bacc6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="f79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000ff"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="ff00ff"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Helvetica Neue" pitchFamily="0" charset="1"/>
+        <a:ea typeface="Helvetica Neue" pitchFamily="0" charset="1"/>
+        <a:cs typeface="Helvetica Neue" pitchFamily="0" charset="1"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Helvetica Neue" pitchFamily="0" charset="1"/>
+        <a:ea typeface="Helvetica Neue" pitchFamily="0" charset="1"/>
+        <a:cs typeface="Helvetica Neue" pitchFamily="0" charset="1"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme>
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+          <a:tileRect l="0" t="0" r="0" b="0"/>
+        </a:gradFill>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+          <a:tileRect l="0" t="0" r="0" b="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+          <a:tileRect l="0" t="0" r="0" b="0"/>
+        </a:gradFill>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+          <a:tileRect l="0" t="0" r="0" b="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
@@ -912,8 +1068,8 @@
   </sheetPr>
   <dimension ref="A1:P10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L1" activeCellId="0" sqref="L1"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H3" activeCellId="0" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -970,13 +1126,13 @@
       <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="N1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="O1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="P1" s="2" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1002,25 +1158,25 @@
       <c r="G2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="I2" s="5"/>
+      <c r="I2" s="4"/>
       <c r="J2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
       <c r="M2" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="N2" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="O2" s="7" t="n">
+      <c r="O2" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="P2" s="8"/>
+      <c r="P2" s="4"/>
     </row>
     <row r="3" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
@@ -1029,7 +1185,7 @@
       <c r="B3" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="5" t="s">
         <v>28</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -1053,157 +1209,157 @@
       <c r="J3" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
       <c r="M3" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="N3" s="3" t="str">
+      <c r="N3" s="2" t="str">
         <f aca="false">RIGHT(H3,LEN(H3)-FIND("@",H3,1))</f>
         <v>shodo.io</v>
       </c>
-      <c r="O3" s="7" t="n">
+      <c r="O3" s="4" t="n">
         <f aca="false">COUNTIF(H1:H10,H3)</f>
         <v>1</v>
       </c>
-      <c r="P3" s="8"/>
+      <c r="P3" s="4"/>
     </row>
     <row r="4" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="5" t="n">
+      <c r="A4" s="4" t="n">
         <v>0</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C4" s="10"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
       <c r="F4" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="G4" s="5"/>
+      <c r="G4" s="4"/>
       <c r="H4" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5"/>
-      <c r="L4" s="5"/>
-      <c r="M4" s="5"/>
-      <c r="N4" s="7"/>
-      <c r="O4" s="7" t="n">
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
+      <c r="N4" s="4"/>
+      <c r="O4" s="4" t="n">
         <f aca="false">COUNTIF(H1:H10,H4)</f>
         <v>1</v>
       </c>
-      <c r="P4" s="8"/>
+      <c r="P4" s="4"/>
     </row>
     <row r="5" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="6"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
-      <c r="L5" s="6"/>
-      <c r="M5" s="6"/>
-      <c r="N5" s="8"/>
-      <c r="O5" s="8"/>
-      <c r="P5" s="8"/>
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="4"/>
+      <c r="N5" s="4"/>
+      <c r="O5" s="4"/>
+      <c r="P5" s="4"/>
     </row>
     <row r="6" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="6"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="6"/>
-      <c r="L6" s="6"/>
-      <c r="M6" s="6"/>
-      <c r="N6" s="8"/>
-      <c r="O6" s="8"/>
-      <c r="P6" s="8"/>
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4"/>
+      <c r="M6" s="4"/>
+      <c r="N6" s="4"/>
+      <c r="O6" s="4"/>
+      <c r="P6" s="4"/>
     </row>
     <row r="7" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="6"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="6"/>
-      <c r="L7" s="6"/>
-      <c r="M7" s="6"/>
-      <c r="N7" s="8"/>
-      <c r="O7" s="8"/>
-      <c r="P7" s="8"/>
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
+      <c r="M7" s="4"/>
+      <c r="N7" s="4"/>
+      <c r="O7" s="4"/>
+      <c r="P7" s="4"/>
     </row>
     <row r="8" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="6"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="6"/>
-      <c r="K8" s="6"/>
-      <c r="L8" s="6"/>
-      <c r="M8" s="6"/>
-      <c r="N8" s="8"/>
-      <c r="O8" s="8"/>
-      <c r="P8" s="8"/>
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="4"/>
+      <c r="N8" s="4"/>
+      <c r="O8" s="4"/>
+      <c r="P8" s="4"/>
     </row>
     <row r="9" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="6"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
-      <c r="K9" s="6"/>
-      <c r="L9" s="6"/>
-      <c r="M9" s="6"/>
-      <c r="N9" s="8"/>
-      <c r="O9" s="8"/>
-      <c r="P9" s="8"/>
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="4"/>
+      <c r="M9" s="4"/>
+      <c r="N9" s="4"/>
+      <c r="O9" s="4"/>
+      <c r="P9" s="4"/>
     </row>
     <row r="10" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="6"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
-      <c r="K10" s="6"/>
-      <c r="L10" s="6"/>
-      <c r="M10" s="6"/>
-      <c r="N10" s="8"/>
-      <c r="O10" s="8"/>
-      <c r="P10" s="8"/>
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="4"/>
+      <c r="M10" s="4"/>
+      <c r="N10" s="4"/>
+      <c r="O10" s="4"/>
+      <c r="P10" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1248,8 +1404,8 @@
       <c r="C1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
@@ -1261,8 +1417,8 @@
       <c r="C2" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
@@ -1274,8 +1430,8 @@
       <c r="C3" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
@@ -1287,8 +1443,8 @@
       <c r="C4" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
@@ -1300,8 +1456,8 @@
       <c r="C5" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
@@ -1313,8 +1469,8 @@
       <c r="C6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
@@ -1326,8 +1482,8 @@
       <c r="C7" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
@@ -1339,8 +1495,8 @@
       <c r="C8" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
@@ -1352,8 +1508,8 @@
       <c r="C9" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
@@ -1365,8 +1521,8 @@
       <c r="C10" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
@@ -1378,8 +1534,8 @@
       <c r="C11" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
@@ -1391,8 +1547,8 @@
       <c r="C12" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
@@ -1404,8 +1560,8 @@
       <c r="C13" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
@@ -1417,8 +1573,8 @@
       <c r="C14" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
@@ -1430,8 +1586,8 @@
       <c r="C15" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
@@ -1443,8 +1599,8 @@
       <c r="C16" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
@@ -1456,8 +1612,8 @@
       <c r="C17" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
@@ -1469,8 +1625,8 @@
       <c r="C18" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
@@ -1482,8 +1638,8 @@
       <c r="C19" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
     </row>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
@@ -1495,8 +1651,8 @@
       <c r="C20" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="s">
@@ -1508,8 +1664,8 @@
       <c r="C21" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="D21" s="8"/>
-      <c r="E21" s="8"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
@@ -1521,8 +1677,8 @@
       <c r="C22" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
     </row>
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
@@ -1534,8 +1690,8 @@
       <c r="C23" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="D23" s="8"/>
-      <c r="E23" s="8"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="s">
@@ -1547,8 +1703,8 @@
       <c r="C24" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="D24" s="8"/>
-      <c r="E24" s="8"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="s">
@@ -1560,8 +1716,8 @@
       <c r="C25" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="D25" s="8"/>
-      <c r="E25" s="8"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
     </row>
     <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="s">
@@ -1573,8 +1729,8 @@
       <c r="C26" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="D26" s="8"/>
-      <c r="E26" s="8"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
     </row>
     <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="s">
@@ -1586,8 +1742,8 @@
       <c r="C27" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="D27" s="8"/>
-      <c r="E27" s="8"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
     </row>
     <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="s">
@@ -1599,8 +1755,8 @@
       <c r="C28" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="D28" s="8"/>
-      <c r="E28" s="8"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="s">
@@ -1612,8 +1768,8 @@
       <c r="C29" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="D29" s="8"/>
-      <c r="E29" s="8"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
     </row>
     <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="2" t="s">
@@ -1625,8 +1781,8 @@
       <c r="C30" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="D30" s="8"/>
-      <c r="E30" s="8"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
     </row>
     <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="s">
@@ -1638,8 +1794,8 @@
       <c r="C31" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="D31" s="8"/>
-      <c r="E31" s="8"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="4"/>
     </row>
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="s">
@@ -1651,8 +1807,8 @@
       <c r="C32" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="D32" s="8"/>
-      <c r="E32" s="8"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="4"/>
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="2" t="s">
@@ -1664,8 +1820,8 @@
       <c r="C33" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="D33" s="8"/>
-      <c r="E33" s="8"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="4"/>
     </row>
     <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="2" t="s">
@@ -1677,8 +1833,8 @@
       <c r="C34" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="D34" s="8"/>
-      <c r="E34" s="8"/>
+      <c r="D34" s="4"/>
+      <c r="E34" s="4"/>
     </row>
     <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="2" t="s">
@@ -1690,8 +1846,8 @@
       <c r="C35" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="D35" s="8"/>
-      <c r="E35" s="8"/>
+      <c r="D35" s="4"/>
+      <c r="E35" s="4"/>
     </row>
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="2" t="s">
@@ -1703,8 +1859,8 @@
       <c r="C36" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="D36" s="8"/>
-      <c r="E36" s="8"/>
+      <c r="D36" s="4"/>
+      <c r="E36" s="4"/>
     </row>
     <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="2" t="s">
@@ -1716,8 +1872,8 @@
       <c r="C37" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="D37" s="8"/>
-      <c r="E37" s="8"/>
+      <c r="D37" s="4"/>
+      <c r="E37" s="4"/>
     </row>
     <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="2" t="s">
@@ -1729,8 +1885,8 @@
       <c r="C38" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="D38" s="8"/>
-      <c r="E38" s="8"/>
+      <c r="D38" s="4"/>
+      <c r="E38" s="4"/>
     </row>
     <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="2" t="s">
@@ -1742,8 +1898,8 @@
       <c r="C39" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="D39" s="8"/>
-      <c r="E39" s="8"/>
+      <c r="D39" s="4"/>
+      <c r="E39" s="4"/>
     </row>
     <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="2" t="s">
@@ -1755,8 +1911,8 @@
       <c r="C40" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="D40" s="8"/>
-      <c r="E40" s="8"/>
+      <c r="D40" s="4"/>
+      <c r="E40" s="4"/>
     </row>
     <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="2" t="s">
@@ -1768,8 +1924,8 @@
       <c r="C41" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="D41" s="8"/>
-      <c r="E41" s="8"/>
+      <c r="D41" s="4"/>
+      <c r="E41" s="4"/>
     </row>
     <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="2" t="s">
@@ -1781,8 +1937,8 @@
       <c r="C42" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="D42" s="8"/>
-      <c r="E42" s="8"/>
+      <c r="D42" s="4"/>
+      <c r="E42" s="4"/>
     </row>
     <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="2" t="s">
@@ -1794,8 +1950,8 @@
       <c r="C43" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="D43" s="8"/>
-      <c r="E43" s="8"/>
+      <c r="D43" s="4"/>
+      <c r="E43" s="4"/>
     </row>
     <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="2" t="s">
@@ -1807,8 +1963,8 @@
       <c r="C44" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="D44" s="8"/>
-      <c r="E44" s="8"/>
+      <c r="D44" s="4"/>
+      <c r="E44" s="4"/>
     </row>
     <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="2" t="s">
@@ -1820,8 +1976,8 @@
       <c r="C45" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="D45" s="8"/>
-      <c r="E45" s="8"/>
+      <c r="D45" s="4"/>
+      <c r="E45" s="4"/>
     </row>
     <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="2" t="s">
@@ -1833,8 +1989,8 @@
       <c r="C46" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="D46" s="8"/>
-      <c r="E46" s="8"/>
+      <c r="D46" s="4"/>
+      <c r="E46" s="4"/>
     </row>
     <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="2" t="s">
@@ -1846,8 +2002,8 @@
       <c r="C47" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="D47" s="8"/>
-      <c r="E47" s="8"/>
+      <c r="D47" s="4"/>
+      <c r="E47" s="4"/>
     </row>
     <row r="48" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="2" t="s">
@@ -1859,8 +2015,8 @@
       <c r="C48" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="D48" s="8"/>
-      <c r="E48" s="8"/>
+      <c r="D48" s="4"/>
+      <c r="E48" s="4"/>
     </row>
     <row r="49" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="2" t="s">
@@ -1872,8 +2028,8 @@
       <c r="C49" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="D49" s="8"/>
-      <c r="E49" s="8"/>
+      <c r="D49" s="4"/>
+      <c r="E49" s="4"/>
     </row>
     <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="2" t="s">
@@ -1885,8 +2041,8 @@
       <c r="C50" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="D50" s="8"/>
-      <c r="E50" s="8"/>
+      <c r="D50" s="4"/>
+      <c r="E50" s="4"/>
     </row>
     <row r="51" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="2" t="s">
@@ -1898,8 +2054,8 @@
       <c r="C51" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="D51" s="8"/>
-      <c r="E51" s="8"/>
+      <c r="D51" s="4"/>
+      <c r="E51" s="4"/>
     </row>
     <row r="52" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="2" t="s">
@@ -1911,8 +2067,8 @@
       <c r="C52" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="D52" s="8"/>
-      <c r="E52" s="8"/>
+      <c r="D52" s="4"/>
+      <c r="E52" s="4"/>
     </row>
     <row r="53" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="2" t="s">
@@ -1924,8 +2080,8 @@
       <c r="C53" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="D53" s="8"/>
-      <c r="E53" s="8"/>
+      <c r="D53" s="4"/>
+      <c r="E53" s="4"/>
     </row>
     <row r="54" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="2" t="s">
@@ -1937,8 +2093,8 @@
       <c r="C54" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="D54" s="8"/>
-      <c r="E54" s="8"/>
+      <c r="D54" s="4"/>
+      <c r="E54" s="4"/>
     </row>
     <row r="55" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="2" t="s">
@@ -1950,8 +2106,8 @@
       <c r="C55" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="D55" s="8"/>
-      <c r="E55" s="8"/>
+      <c r="D55" s="4"/>
+      <c r="E55" s="4"/>
     </row>
     <row r="56" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="2" t="s">
@@ -1963,8 +2119,8 @@
       <c r="C56" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="D56" s="8"/>
-      <c r="E56" s="8"/>
+      <c r="D56" s="4"/>
+      <c r="E56" s="4"/>
     </row>
     <row r="57" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="2" t="s">
@@ -1976,8 +2132,8 @@
       <c r="C57" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="D57" s="8"/>
-      <c r="E57" s="8"/>
+      <c r="D57" s="4"/>
+      <c r="E57" s="4"/>
     </row>
     <row r="58" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="2" t="s">
@@ -1989,8 +2145,8 @@
       <c r="C58" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="D58" s="8"/>
-      <c r="E58" s="8"/>
+      <c r="D58" s="4"/>
+      <c r="E58" s="4"/>
     </row>
     <row r="59" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="2" t="s">
@@ -2002,8 +2158,8 @@
       <c r="C59" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="D59" s="8"/>
-      <c r="E59" s="8"/>
+      <c r="D59" s="4"/>
+      <c r="E59" s="4"/>
     </row>
     <row r="60" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="2" t="s">
@@ -2015,8 +2171,8 @@
       <c r="C60" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="D60" s="8"/>
-      <c r="E60" s="8"/>
+      <c r="D60" s="4"/>
+      <c r="E60" s="4"/>
     </row>
     <row r="61" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="2" t="s">
@@ -2028,8 +2184,8 @@
       <c r="C61" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="D61" s="8"/>
-      <c r="E61" s="8"/>
+      <c r="D61" s="4"/>
+      <c r="E61" s="4"/>
     </row>
     <row r="62" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="2" t="s">
@@ -2041,8 +2197,8 @@
       <c r="C62" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="D62" s="8"/>
-      <c r="E62" s="8"/>
+      <c r="D62" s="4"/>
+      <c r="E62" s="4"/>
     </row>
     <row r="63" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="2" t="s">
@@ -2054,8 +2210,8 @@
       <c r="C63" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="D63" s="8"/>
-      <c r="E63" s="8"/>
+      <c r="D63" s="4"/>
+      <c r="E63" s="4"/>
     </row>
     <row r="64" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="2" t="s">
@@ -2067,8 +2223,8 @@
       <c r="C64" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="D64" s="8"/>
-      <c r="E64" s="8"/>
+      <c r="D64" s="4"/>
+      <c r="E64" s="4"/>
     </row>
     <row r="65" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="2" t="s">
@@ -2080,8 +2236,8 @@
       <c r="C65" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="D65" s="8"/>
-      <c r="E65" s="8"/>
+      <c r="D65" s="4"/>
+      <c r="E65" s="4"/>
     </row>
     <row r="66" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="2" t="s">
@@ -2093,8 +2249,8 @@
       <c r="C66" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="D66" s="8"/>
-      <c r="E66" s="8"/>
+      <c r="D66" s="4"/>
+      <c r="E66" s="4"/>
     </row>
     <row r="67" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="2" t="s">
@@ -2106,8 +2262,8 @@
       <c r="C67" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="D67" s="8"/>
-      <c r="E67" s="8"/>
+      <c r="D67" s="4"/>
+      <c r="E67" s="4"/>
     </row>
     <row r="68" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A68" s="2" t="s">
@@ -2119,8 +2275,8 @@
       <c r="C68" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="D68" s="8"/>
-      <c r="E68" s="8"/>
+      <c r="D68" s="4"/>
+      <c r="E68" s="4"/>
     </row>
     <row r="69" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="2" t="s">
@@ -2132,8 +2288,8 @@
       <c r="C69" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="D69" s="8"/>
-      <c r="E69" s="8"/>
+      <c r="D69" s="4"/>
+      <c r="E69" s="4"/>
     </row>
     <row r="70" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="2" t="s">
@@ -2145,8 +2301,8 @@
       <c r="C70" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="D70" s="8"/>
-      <c r="E70" s="8"/>
+      <c r="D70" s="4"/>
+      <c r="E70" s="4"/>
     </row>
     <row r="71" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="2" t="s">
@@ -2158,8 +2314,8 @@
       <c r="C71" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="D71" s="8"/>
-      <c r="E71" s="8"/>
+      <c r="D71" s="4"/>
+      <c r="E71" s="4"/>
     </row>
     <row r="72" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="2" t="s">
@@ -2171,8 +2327,8 @@
       <c r="C72" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="D72" s="8"/>
-      <c r="E72" s="8"/>
+      <c r="D72" s="4"/>
+      <c r="E72" s="4"/>
     </row>
     <row r="73" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="2" t="s">
@@ -2184,8 +2340,8 @@
       <c r="C73" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="D73" s="8"/>
-      <c r="E73" s="8"/>
+      <c r="D73" s="4"/>
+      <c r="E73" s="4"/>
     </row>
     <row r="74" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="2" t="s">
@@ -2197,8 +2353,8 @@
       <c r="C74" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="D74" s="8"/>
-      <c r="E74" s="8"/>
+      <c r="D74" s="4"/>
+      <c r="E74" s="4"/>
     </row>
     <row r="75" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="2" t="s">
@@ -2210,8 +2366,8 @@
       <c r="C75" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="D75" s="8"/>
-      <c r="E75" s="8"/>
+      <c r="D75" s="4"/>
+      <c r="E75" s="4"/>
     </row>
     <row r="76" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="2" t="s">
@@ -2223,8 +2379,8 @@
       <c r="C76" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="D76" s="8"/>
-      <c r="E76" s="8"/>
+      <c r="D76" s="4"/>
+      <c r="E76" s="4"/>
     </row>
     <row r="77" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A77" s="2" t="s">
@@ -2236,8 +2392,8 @@
       <c r="C77" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="D77" s="8"/>
-      <c r="E77" s="8"/>
+      <c r="D77" s="4"/>
+      <c r="E77" s="4"/>
     </row>
     <row r="78" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="2" t="s">
@@ -2249,8 +2405,8 @@
       <c r="C78" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="D78" s="8"/>
-      <c r="E78" s="8"/>
+      <c r="D78" s="4"/>
+      <c r="E78" s="4"/>
     </row>
     <row r="79" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A79" s="2" t="s">
@@ -2262,8 +2418,8 @@
       <c r="C79" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="D79" s="8"/>
-      <c r="E79" s="8"/>
+      <c r="D79" s="4"/>
+      <c r="E79" s="4"/>
     </row>
     <row r="80" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A80" s="2" t="s">
@@ -2275,8 +2431,8 @@
       <c r="C80" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="D80" s="8"/>
-      <c r="E80" s="8"/>
+      <c r="D80" s="4"/>
+      <c r="E80" s="4"/>
     </row>
     <row r="81" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A81" s="2" t="s">
@@ -2288,8 +2444,8 @@
       <c r="C81" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="D81" s="8"/>
-      <c r="E81" s="8"/>
+      <c r="D81" s="4"/>
+      <c r="E81" s="4"/>
     </row>
     <row r="82" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A82" s="2" t="s">
@@ -2301,8 +2457,8 @@
       <c r="C82" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="D82" s="8"/>
-      <c r="E82" s="8"/>
+      <c r="D82" s="4"/>
+      <c r="E82" s="4"/>
     </row>
     <row r="83" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A83" s="2" t="s">
@@ -2314,8 +2470,8 @@
       <c r="C83" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="D83" s="8"/>
-      <c r="E83" s="8"/>
+      <c r="D83" s="4"/>
+      <c r="E83" s="4"/>
     </row>
     <row r="84" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A84" s="2" t="s">
@@ -2327,8 +2483,8 @@
       <c r="C84" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="D84" s="8"/>
-      <c r="E84" s="8"/>
+      <c r="D84" s="4"/>
+      <c r="E84" s="4"/>
     </row>
     <row r="85" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A85" s="2" t="s">
@@ -2340,8 +2496,8 @@
       <c r="C85" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="D85" s="8"/>
-      <c r="E85" s="8"/>
+      <c r="D85" s="4"/>
+      <c r="E85" s="4"/>
     </row>
     <row r="86" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A86" s="2" t="s">
@@ -2353,8 +2509,8 @@
       <c r="C86" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="D86" s="8"/>
-      <c r="E86" s="8"/>
+      <c r="D86" s="4"/>
+      <c r="E86" s="4"/>
     </row>
     <row r="87" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A87" s="2" t="s">
@@ -2366,8 +2522,8 @@
       <c r="C87" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="D87" s="8"/>
-      <c r="E87" s="8"/>
+      <c r="D87" s="4"/>
+      <c r="E87" s="4"/>
     </row>
     <row r="88" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A88" s="2" t="s">
@@ -2379,8 +2535,8 @@
       <c r="C88" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="D88" s="8"/>
-      <c r="E88" s="8"/>
+      <c r="D88" s="4"/>
+      <c r="E88" s="4"/>
     </row>
     <row r="89" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A89" s="2" t="s">
@@ -2392,8 +2548,8 @@
       <c r="C89" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="D89" s="8"/>
-      <c r="E89" s="8"/>
+      <c r="D89" s="4"/>
+      <c r="E89" s="4"/>
     </row>
     <row r="90" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A90" s="2" t="s">
@@ -2405,8 +2561,8 @@
       <c r="C90" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="D90" s="8"/>
-      <c r="E90" s="8"/>
+      <c r="D90" s="4"/>
+      <c r="E90" s="4"/>
     </row>
     <row r="91" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A91" s="2" t="s">
@@ -2418,8 +2574,8 @@
       <c r="C91" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="D91" s="8"/>
-      <c r="E91" s="8"/>
+      <c r="D91" s="4"/>
+      <c r="E91" s="4"/>
     </row>
     <row r="92" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A92" s="2" t="s">
@@ -2431,8 +2587,8 @@
       <c r="C92" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="D92" s="8"/>
-      <c r="E92" s="8"/>
+      <c r="D92" s="4"/>
+      <c r="E92" s="4"/>
     </row>
     <row r="93" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A93" s="2" t="s">
@@ -2444,8 +2600,8 @@
       <c r="C93" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="D93" s="8"/>
-      <c r="E93" s="8"/>
+      <c r="D93" s="4"/>
+      <c r="E93" s="4"/>
     </row>
     <row r="94" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A94" s="2" t="s">
@@ -2457,8 +2613,8 @@
       <c r="C94" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="D94" s="8"/>
-      <c r="E94" s="8"/>
+      <c r="D94" s="4"/>
+      <c r="E94" s="4"/>
     </row>
     <row r="95" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A95" s="2" t="s">
@@ -2470,8 +2626,8 @@
       <c r="C95" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="D95" s="8"/>
-      <c r="E95" s="8"/>
+      <c r="D95" s="4"/>
+      <c r="E95" s="4"/>
     </row>
     <row r="96" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A96" s="2" t="s">
@@ -2483,8 +2639,8 @@
       <c r="C96" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="D96" s="8"/>
-      <c r="E96" s="8"/>
+      <c r="D96" s="4"/>
+      <c r="E96" s="4"/>
     </row>
     <row r="97" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A97" s="2" t="s">
@@ -2496,8 +2652,8 @@
       <c r="C97" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="D97" s="8"/>
-      <c r="E97" s="8"/>
+      <c r="D97" s="4"/>
+      <c r="E97" s="4"/>
     </row>
     <row r="98" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A98" s="2" t="s">
@@ -2509,8 +2665,8 @@
       <c r="C98" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="D98" s="8"/>
-      <c r="E98" s="8"/>
+      <c r="D98" s="4"/>
+      <c r="E98" s="4"/>
     </row>
     <row r="99" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A99" s="2" t="s">
@@ -2522,8 +2678,8 @@
       <c r="C99" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="D99" s="8"/>
-      <c r="E99" s="8"/>
+      <c r="D99" s="4"/>
+      <c r="E99" s="4"/>
     </row>
     <row r="100" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A100" s="2" t="s">
@@ -2535,8 +2691,8 @@
       <c r="C100" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="D100" s="8"/>
-      <c r="E100" s="8"/>
+      <c r="D100" s="4"/>
+      <c r="E100" s="4"/>
     </row>
     <row r="101" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A101" s="2" t="s">
@@ -2548,8 +2704,8 @@
       <c r="C101" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="D101" s="8"/>
-      <c r="E101" s="8"/>
+      <c r="D101" s="4"/>
+      <c r="E101" s="4"/>
     </row>
     <row r="102" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A102" s="2" t="s">
@@ -2561,8 +2717,8 @@
       <c r="C102" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="D102" s="8"/>
-      <c r="E102" s="8"/>
+      <c r="D102" s="4"/>
+      <c r="E102" s="4"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2595,297 +2751,297 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="8"/>
-      <c r="B1" s="3" t="s">
+      <c r="A1" s="4"/>
+      <c r="B1" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
     </row>
     <row r="2" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
     </row>
     <row r="3" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
     </row>
     <row r="4" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
     </row>
     <row r="5" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
     </row>
     <row r="6" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
     </row>
     <row r="7" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
     </row>
     <row r="8" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
     </row>
     <row r="9" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
     </row>
     <row r="10" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
     </row>
     <row r="11" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
     </row>
     <row r="12" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
     </row>
     <row r="13" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
     </row>
     <row r="14" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
     </row>
     <row r="15" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
     </row>
     <row r="16" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
     </row>
     <row r="17" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
     </row>
     <row r="18" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C18" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
     </row>
     <row r="19" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="3" t="s">
+      <c r="A19" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="2" t="s">
         <v>230</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C19" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
     </row>
     <row r="20" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="3" t="s">
+      <c r="A20" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C20" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
     </row>
     <row r="21" customFormat="false" ht="78" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="3" t="s">
+      <c r="A21" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="B21" s="11" t="s">
+      <c r="B21" s="7" t="s">
         <v>236</v>
       </c>
-      <c r="C21" s="11" t="s">
+      <c r="C21" s="7" t="s">
         <v>237</v>
       </c>
-      <c r="D21" s="8"/>
-      <c r="E21" s="8"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
     </row>
     <row r="22" customFormat="false" ht="14" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="3" t="s">
+      <c r="A22" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="B22" s="11" t="s">
+      <c r="B22" s="7" t="s">
         <v>239</v>
       </c>
-      <c r="C22" s="8"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
     </row>
     <row r="23" customFormat="false" ht="14" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="3" t="s">
+      <c r="A23" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="B23" s="11" t="s">
+      <c r="B23" s="7" t="s">
         <v>241</v>
       </c>
-      <c r="C23" s="8"/>
-      <c r="D23" s="8"/>
-      <c r="E23" s="8"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>